<commit_message>
add two weeks develop plan
</commit_message>
<xml_diff>
--- a/design/favorites_2.0 开发计划.xlsx
+++ b/design/favorites_2.0 开发计划.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15870" windowHeight="9390"/>
+    <workbookView windowWidth="15870" windowHeight="8970"/>
   </bookViews>
   <sheets>
     <sheet name="开发清单" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94">
   <si>
     <t>项目名称</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>YanceyYu</t>
+  </si>
+  <si>
+    <t>已投SIT</t>
   </si>
   <si>
     <t>随便看看</t>
@@ -125,6 +128,15 @@
     <t>TangPetty</t>
   </si>
   <si>
+    <t>2017/1/23 2017/2/15</t>
+  </si>
+  <si>
+    <t>预计2月15日完成</t>
+  </si>
+  <si>
+    <t>由于工作量大、逻辑比较复杂该需求进度延期到2月15日完成</t>
+  </si>
+  <si>
     <t>个人主页</t>
   </si>
   <si>
@@ -153,9 +165,6 @@
 2）增加一个上传背景图的按钮用户通过点击按钮上传一张自定义背景图片；</t>
   </si>
   <si>
-    <t>已完成</t>
-  </si>
-  <si>
     <t>私信小纸条</t>
   </si>
   <si>
@@ -211,6 +220,9 @@
     <t>分享功能</t>
   </si>
   <si>
+    <t>分享收藏文章</t>
+  </si>
+  <si>
     <t>用户可以把云收藏上面的文章分享到各大社区</t>
   </si>
   <si>
@@ -224,6 +236,9 @@
   </si>
   <si>
     <t>用户登录的时候可以选择QQ、微博、微信授权登录</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Smilence1024 </t>
   </si>
   <si>
     <t>意见反馈</t>
@@ -263,9 +278,6 @@
     <t>优化</t>
   </si>
   <si>
-    <t xml:space="preserve">Smilence1024 </t>
-  </si>
-  <si>
     <t>处理文章中logo是空的选项（定时）</t>
   </si>
   <si>
@@ -288,6 +300,21 @@
   </si>
   <si>
     <t>ityouknow</t>
+  </si>
+  <si>
+    <t>更改图片</t>
+  </si>
+  <si>
+    <t>更改用户默认头像和网页标题logo</t>
+  </si>
+  <si>
+    <t>将原有的默认头像和网页标题logo改为新的</t>
+  </si>
+  <si>
+    <t>易</t>
+  </si>
+  <si>
+    <t>小</t>
   </si>
   <si>
     <t>备注：以上列表中出现15个字符以上内容均用“...”代替</t>
@@ -299,8 +326,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
@@ -319,21 +346,14 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -344,32 +364,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -392,7 +388,29 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -403,20 +421,6 @@
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -436,16 +440,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -453,7 +449,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -466,6 +470,29 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -488,25 +515,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -518,60 +617,66 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -584,91 +689,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -679,30 +706,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -717,6 +720,50 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -745,37 +792,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -784,148 +811,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -941,6 +968,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -959,7 +989,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -984,7 +1014,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
@@ -1008,9 +1038,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1398,22 +1425,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:P20"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="N5" sqref="N5"/>
+      <selection pane="bottomLeft" activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="11" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5" style="4" customWidth="1"/>
-    <col min="3" max="3" width="11" style="4" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="5" customWidth="1"/>
+    <col min="3" max="3" width="11" style="5" customWidth="1"/>
     <col min="4" max="4" width="13" style="1" customWidth="1"/>
     <col min="5" max="5" width="28" style="1" customWidth="1"/>
-    <col min="6" max="6" width="31.625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="31.625" style="6" customWidth="1"/>
     <col min="7" max="7" width="11" style="1" customWidth="1"/>
     <col min="8" max="9" width="9.125" style="1" customWidth="1"/>
     <col min="10" max="14" width="11" style="1" customWidth="1"/>
@@ -1423,72 +1450,72 @@
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="1" spans="1:16">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="20" t="s">
+      <c r="O1" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="21" t="s">
+      <c r="P1" s="22" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" ht="108" spans="1:15">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="14" t="s">
         <v>21</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -1500,76 +1527,82 @@
       <c r="I2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="22" t="s">
+      <c r="J2" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="23" t="s">
+      <c r="K2" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="24">
+      <c r="L2" s="25">
         <v>42751</v>
       </c>
-      <c r="M2" s="24">
+      <c r="M2" s="25">
         <v>42764</v>
       </c>
-      <c r="N2" s="12"/>
-      <c r="O2" s="23"/>
+      <c r="N2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" s="24"/>
     </row>
     <row r="3" ht="202.5" spans="1:15">
-      <c r="A3" s="9"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="12" t="s">
+      <c r="A3" s="10"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="D3" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="E3" s="13" t="s">
         <v>29</v>
       </c>
+      <c r="F3" s="14" t="s">
+        <v>30</v>
+      </c>
       <c r="G3" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="L3" s="24">
+      <c r="K3" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="25">
         <v>42754</v>
       </c>
-      <c r="M3" s="24">
-        <v>42758</v>
-      </c>
-      <c r="N3" s="22"/>
-      <c r="O3" s="23"/>
+      <c r="M3" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="N3" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" s="24" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="4" s="3" customFormat="1" ht="67.5" spans="1:13">
-      <c r="A4" s="9"/>
-      <c r="B4" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>34</v>
+    <row r="4" s="3" customFormat="1" ht="67.5" spans="1:14">
+      <c r="A4" s="10"/>
+      <c r="B4" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>36</v>
+        <v>39</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>40</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>22</v>
@@ -1580,33 +1613,36 @@
       <c r="I4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="L4" s="24">
+      <c r="K4" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" s="25">
         <v>42751</v>
       </c>
-      <c r="M4" s="24">
+      <c r="M4" s="25">
         <v>42753</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="5" s="3" customFormat="1" ht="67.5" spans="1:14">
-      <c r="A5" s="9"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="10" t="s">
-        <v>37</v>
+      <c r="A5" s="10"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="11" t="s">
+        <v>41</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>40</v>
+        <v>43</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>44</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>22</v>
@@ -1617,36 +1653,36 @@
       <c r="I5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="J5" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="K5" s="23" t="s">
+      <c r="K5" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="L5" s="24">
+      <c r="L5" s="25">
         <v>42755</v>
       </c>
-      <c r="M5" s="24">
+      <c r="M5" s="25">
         <v>42758</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" s="3" customFormat="1" ht="67.5" spans="1:13">
-      <c r="A6" s="9"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="10" t="s">
-        <v>42</v>
+      <c r="A6" s="10"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>44</v>
+        <v>46</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>47</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>22</v>
@@ -1657,60 +1693,60 @@
       <c r="I6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="J6" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="K6" s="23"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
     </row>
     <row r="7" s="3" customFormat="1" ht="94.5" spans="1:13">
-      <c r="A7" s="9"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="10" t="s">
-        <v>45</v>
+      <c r="A7" s="10"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>47</v>
+        <v>49</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>50</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>22</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J7" s="12" t="s">
+      <c r="J7" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="K7" s="23"/>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
     </row>
     <row r="8" s="3" customFormat="1" ht="81" spans="1:13">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>49</v>
+      <c r="A8" s="10"/>
+      <c r="B8" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>52</v>
+        <v>54</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>55</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>22</v>
@@ -1721,28 +1757,35 @@
       <c r="I8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="12" t="s">
+      <c r="J8" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25"/>
+      <c r="K8" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="L8" s="25">
+        <v>42779</v>
+      </c>
+      <c r="M8" s="25">
+        <v>42783</v>
+      </c>
     </row>
     <row r="9" s="3" customFormat="1" ht="27" spans="1:13">
-      <c r="A9" s="9"/>
-      <c r="B9" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>54</v>
+      <c r="A9" s="10"/>
+      <c r="B9" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>57</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>56</v>
+        <v>58</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>59</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>22</v>
@@ -1753,27 +1796,36 @@
       <c r="I9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J9" s="12" t="s">
+      <c r="J9" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="K9" s="23"/>
-      <c r="L9" s="24"/>
-      <c r="M9" s="24"/>
+      <c r="K9" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="L9" s="25">
+        <v>42782</v>
+      </c>
+      <c r="M9" s="25">
+        <v>42786</v>
+      </c>
     </row>
     <row r="10" s="3" customFormat="1" ht="40.5" spans="1:13">
-      <c r="A10" s="9"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="10" t="s">
-        <v>57</v>
+      <c r="A10" s="10"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="G10" s="17" t="s">
-        <v>30</v>
+        <v>62</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>22</v>
@@ -1781,32 +1833,38 @@
       <c r="I10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J10" s="12" t="s">
+      <c r="J10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="K10" s="23"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="24"/>
+      <c r="K10" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="L10" s="25">
+        <v>42786</v>
+      </c>
+      <c r="M10" s="25">
+        <v>42790</v>
+      </c>
     </row>
     <row r="11" s="3" customFormat="1" ht="27" spans="1:13">
-      <c r="A11" s="9"/>
-      <c r="B11" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>61</v>
+      <c r="A11" s="10"/>
+      <c r="B11" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>65</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="G11" s="17" t="s">
-        <v>30</v>
+        <v>66</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>22</v>
@@ -1814,31 +1872,37 @@
       <c r="I11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J11" s="12" t="s">
+      <c r="J11" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="K11" s="23"/>
-      <c r="L11" s="24"/>
-      <c r="M11" s="24"/>
+      <c r="K11" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="L11" s="25">
+        <v>42786</v>
+      </c>
+      <c r="M11" s="25">
+        <v>42790</v>
+      </c>
     </row>
     <row r="12" s="3" customFormat="1" ht="40.5" spans="1:13">
-      <c r="A12" s="9"/>
-      <c r="B12" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>63</v>
+      <c r="A12" s="10"/>
+      <c r="B12" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>68</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="G12" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>22</v>
       </c>
       <c r="H12" s="1" t="s">
@@ -1847,62 +1911,74 @@
       <c r="I12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J12" s="12" t="s">
+      <c r="J12" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="K12" s="23"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="24"/>
+      <c r="K12" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="L12" s="25">
+        <v>42787</v>
+      </c>
+      <c r="M12" s="25">
+        <v>42790</v>
+      </c>
     </row>
     <row r="13" s="3" customFormat="1" ht="40.5" spans="1:13">
-      <c r="A13" s="9"/>
-      <c r="B13" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="C13" s="10" t="s">
+      <c r="A13" s="10"/>
+      <c r="B13" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="K13" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="D13" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="G13" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J13" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="K13" s="23"/>
-      <c r="L13" s="24"/>
-      <c r="M13" s="24"/>
+      <c r="L13" s="25">
+        <v>42779</v>
+      </c>
+      <c r="M13" s="25">
+        <v>42783</v>
+      </c>
     </row>
     <row r="14" s="3" customFormat="1" ht="54" spans="1:14">
-      <c r="A14" s="9"/>
-      <c r="B14" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>71</v>
+      <c r="A14" s="10"/>
+      <c r="B14" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>76</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>73</v>
+        <v>77</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>78</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>22</v>
@@ -1913,67 +1989,76 @@
       <c r="I14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J14" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="K14" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="L14" s="24">
+      <c r="J14" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="K14" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="L14" s="25">
         <v>42746</v>
       </c>
-      <c r="M14" s="24">
+      <c r="M14" s="25">
         <v>42747</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="15" s="3" customFormat="1" ht="54" spans="1:13">
-      <c r="A15" s="9"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="10" t="s">
-        <v>76</v>
+    <row r="15" s="3" customFormat="1" ht="54" spans="1:14">
+      <c r="A15" s="10"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="11" t="s">
+        <v>80</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F15" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J15" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J15" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="K15" s="23"/>
-      <c r="L15" s="24"/>
-      <c r="M15" s="24"/>
+      <c r="K15" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="L15" s="25">
+        <v>42773</v>
+      </c>
+      <c r="M15" s="25">
+        <v>42776</v>
+      </c>
+      <c r="N15" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="16" s="3" customFormat="1" ht="40.5" spans="1:14">
-      <c r="A16" s="9"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="10" t="s">
-        <v>80</v>
+      <c r="A16" s="10"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="11" t="s">
+        <v>84</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>82</v>
+        <v>85</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>86</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>22</v>
@@ -1984,84 +2069,126 @@
       <c r="I16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J16" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="K16" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="L16" s="24">
+      <c r="J16" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="K16" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="L16" s="25">
         <v>42747</v>
       </c>
-      <c r="M16" s="24">
+      <c r="M16" s="25">
         <v>42747</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="18"/>
+    <row r="17" s="4" customFormat="1" ht="40.5" spans="1:14">
+      <c r="A17" s="10"/>
+      <c r="B17" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J17" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="K17" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="L17" s="25">
+        <v>42772</v>
+      </c>
+      <c r="M17" s="25">
+        <v>42772</v>
+      </c>
+      <c r="N17" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="18" spans="1:15">
-      <c r="A18" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
+    <row r="18" spans="1:1">
+      <c r="A18" s="19"/>
     </row>
     <row r="19" spans="1:15">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
+      <c r="A19" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
     </row>
     <row r="20" spans="1:15">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:N16"/>
   <mergeCells count="6">
-    <mergeCell ref="A2:A16"/>
+    <mergeCell ref="A2:A17"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="B4:B7"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="B14:B16"/>
-    <mergeCell ref="A18:O20"/>
+    <mergeCell ref="A19:O21"/>
   </mergeCells>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>